<commit_message>
Load Instructions modified in Encoder to allow access to more memory locations: 0 - 2^15; Added functions to Memory to search, Insert and fetch using LRU and exclusive policy
</commit_message>
<xml_diff>
--- a/phase3/Testing/P3.xlsx
+++ b/phase3/Testing/P3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORK\IIT TP\4th Sem\Computer Organization\Project\phase3\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46DB2360-B997-41A1-82C1-36AEA389CB0C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A889AA7-3F8D-4D43-82E6-9A162BC9B815}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="11">
   <si>
     <t>Stall</t>
   </si>
@@ -117,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,6 +140,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -318,6 +325,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -600,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U262"/>
+  <dimension ref="A1:U302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K264" sqref="K264"/>
+    <sheetView topLeftCell="A282" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B304" sqref="B304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5371,11 +5384,9 @@
         <v>4</v>
       </c>
       <c r="J168" s="24">
-        <v>4</v>
-      </c>
-      <c r="K168" s="22">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="K168" s="22"/>
       <c r="L168" s="22"/>
       <c r="M168" s="22"/>
       <c r="N168" s="22"/>
@@ -5409,11 +5420,9 @@
         <v>4</v>
       </c>
       <c r="K169" s="24">
-        <v>4</v>
-      </c>
-      <c r="L169" s="22">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="L169" s="22"/>
       <c r="M169" s="22"/>
       <c r="N169" s="22"/>
       <c r="O169" s="22"/>
@@ -6603,24 +6612,22 @@
       <c r="G210" s="17">
         <v>1</v>
       </c>
-      <c r="H210" s="17" t="s">
+      <c r="H210" s="17">
         <v>2</v>
       </c>
       <c r="I210" s="17" t="s">
         <v>1</v>
       </c>
       <c r="J210" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K210" s="17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L210" s="17">
-        <v>4</v>
-      </c>
-      <c r="M210" s="9">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M210" s="9"/>
       <c r="N210" s="9"/>
       <c r="O210" s="9"/>
       <c r="P210" s="9"/>
@@ -6640,25 +6647,25 @@
       <c r="E211" s="9"/>
       <c r="F211" s="9"/>
       <c r="G211" s="9"/>
-      <c r="H211" s="9"/>
+      <c r="H211" s="9">
+        <v>1</v>
+      </c>
       <c r="I211" s="9" t="s">
         <v>1</v>
       </c>
       <c r="J211" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K211" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L211" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M211" s="9">
-        <v>4</v>
-      </c>
-      <c r="N211" s="9">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="N211" s="9"/>
       <c r="O211" s="9"/>
       <c r="P211" s="9"/>
       <c r="Q211" s="9"/>
@@ -6681,22 +6688,22 @@
       <c r="I212" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J212" s="9"/>
+      <c r="J212" s="9">
+        <v>1</v>
+      </c>
       <c r="K212" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L212" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M212" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N212" s="9">
-        <v>4</v>
-      </c>
-      <c r="O212" s="9">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="O212" s="9"/>
       <c r="P212" s="9"/>
       <c r="Q212" s="9"/>
       <c r="R212" s="9"/>
@@ -7707,24 +7714,22 @@
       <c r="G248" s="33">
         <v>1</v>
       </c>
-      <c r="H248" s="33" t="s">
+      <c r="H248" s="33">
         <v>2</v>
       </c>
       <c r="I248" s="33" t="s">
         <v>1</v>
       </c>
       <c r="J248" s="33">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K248" s="33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L248" s="33">
-        <v>4</v>
-      </c>
-      <c r="M248" s="33">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M248" s="22"/>
       <c r="N248" s="9"/>
       <c r="O248" s="9"/>
       <c r="P248" s="9"/>
@@ -7744,28 +7749,28 @@
       <c r="E249" s="9"/>
       <c r="F249" s="9"/>
       <c r="G249" s="9"/>
-      <c r="H249" s="9"/>
+      <c r="H249" s="9" t="s">
+        <v>4</v>
+      </c>
       <c r="I249" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="J249" s="9" t="s">
-        <v>4</v>
+      <c r="J249" s="9">
+        <v>1</v>
       </c>
       <c r="K249" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L249" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M249" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N249" s="9">
-        <v>4</v>
-      </c>
-      <c r="O249" s="9">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="O249" s="9"/>
       <c r="P249" s="9"/>
       <c r="Q249" s="9"/>
       <c r="R249" s="9"/>
@@ -7788,22 +7793,22 @@
         <v>1</v>
       </c>
       <c r="J250" s="9"/>
-      <c r="K250" s="9"/>
+      <c r="K250" s="9">
+        <v>1</v>
+      </c>
       <c r="L250" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M250" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N250" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O250" s="9">
-        <v>4</v>
-      </c>
-      <c r="P250" s="9">
-        <v>5</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="P250" s="9"/>
       <c r="Q250" s="9"/>
       <c r="R250" s="9"/>
       <c r="S250" s="9"/>
@@ -8168,8 +8173,2299 @@
       <c r="T262" s="9"/>
       <c r="U262" s="9"/>
     </row>
+    <row r="266" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A266" s="30">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="267" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A267" s="1"/>
+      <c r="B267" s="2">
+        <v>1</v>
+      </c>
+      <c r="C267" s="3">
+        <v>2</v>
+      </c>
+      <c r="D267" s="3">
+        <v>3</v>
+      </c>
+      <c r="E267" s="3">
+        <v>4</v>
+      </c>
+      <c r="F267" s="3">
+        <v>5</v>
+      </c>
+      <c r="G267" s="3">
+        <v>6</v>
+      </c>
+      <c r="H267" s="3">
+        <v>7</v>
+      </c>
+      <c r="I267" s="3">
+        <v>8</v>
+      </c>
+      <c r="J267" s="3">
+        <v>9</v>
+      </c>
+      <c r="K267" s="3">
+        <v>10</v>
+      </c>
+      <c r="L267" s="3">
+        <v>11</v>
+      </c>
+      <c r="M267" s="3">
+        <v>12</v>
+      </c>
+      <c r="N267" s="3">
+        <v>13</v>
+      </c>
+      <c r="O267" s="3">
+        <v>14</v>
+      </c>
+      <c r="P267" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q267" s="3">
+        <v>16</v>
+      </c>
+      <c r="R267" s="3">
+        <v>17</v>
+      </c>
+      <c r="S267" s="3">
+        <v>18</v>
+      </c>
+      <c r="T267" s="3">
+        <v>19</v>
+      </c>
+      <c r="U267" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="268" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A268" s="4">
+        <v>0</v>
+      </c>
+      <c r="B268" s="5">
+        <v>1</v>
+      </c>
+      <c r="C268" s="6">
+        <v>2</v>
+      </c>
+      <c r="D268" s="6">
+        <v>3</v>
+      </c>
+      <c r="E268" s="6">
+        <v>4</v>
+      </c>
+      <c r="F268" s="6">
+        <v>5</v>
+      </c>
+      <c r="G268" s="6"/>
+      <c r="H268" s="6"/>
+      <c r="I268" s="6"/>
+      <c r="J268" s="6"/>
+      <c r="K268" s="6"/>
+      <c r="L268" s="6"/>
+      <c r="M268" s="6"/>
+      <c r="N268" s="6"/>
+      <c r="O268" s="6"/>
+      <c r="P268" s="6"/>
+      <c r="Q268" s="6"/>
+      <c r="R268" s="6"/>
+      <c r="S268" s="6"/>
+      <c r="T268" s="6"/>
+      <c r="U268" s="6"/>
+    </row>
+    <row r="269" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A269" s="7">
+        <v>1</v>
+      </c>
+      <c r="B269" s="8"/>
+      <c r="C269" s="5">
+        <v>1</v>
+      </c>
+      <c r="D269" s="6">
+        <v>2</v>
+      </c>
+      <c r="E269" s="6">
+        <v>3</v>
+      </c>
+      <c r="F269" s="6">
+        <v>4</v>
+      </c>
+      <c r="G269" s="6">
+        <v>5</v>
+      </c>
+      <c r="H269" s="9"/>
+      <c r="I269" s="9"/>
+      <c r="J269" s="9"/>
+      <c r="K269" s="9"/>
+      <c r="L269" s="9"/>
+      <c r="M269" s="9"/>
+      <c r="N269" s="9"/>
+      <c r="O269" s="9"/>
+      <c r="P269" s="9"/>
+      <c r="Q269" s="9"/>
+      <c r="R269" s="9"/>
+      <c r="S269" s="9"/>
+      <c r="T269" s="9"/>
+      <c r="U269" s="9"/>
+    </row>
+    <row r="270" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A270" s="7">
+        <v>2</v>
+      </c>
+      <c r="B270" s="8"/>
+      <c r="C270" s="9"/>
+      <c r="D270" s="5">
+        <v>1</v>
+      </c>
+      <c r="E270" s="6">
+        <v>2</v>
+      </c>
+      <c r="F270" s="6">
+        <v>3</v>
+      </c>
+      <c r="G270" s="6">
+        <v>4</v>
+      </c>
+      <c r="H270" s="6">
+        <v>5</v>
+      </c>
+      <c r="I270" s="9"/>
+      <c r="J270" s="9"/>
+      <c r="K270" s="9"/>
+      <c r="L270" s="9"/>
+      <c r="M270" s="9"/>
+      <c r="N270" s="9"/>
+      <c r="O270" s="9"/>
+      <c r="P270" s="9"/>
+      <c r="Q270" s="9"/>
+      <c r="R270" s="9"/>
+      <c r="S270" s="9"/>
+      <c r="T270" s="9"/>
+      <c r="U270" s="9"/>
+    </row>
+    <row r="271" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A271" s="7">
+        <v>3</v>
+      </c>
+      <c r="B271" s="8"/>
+      <c r="C271" s="9"/>
+      <c r="D271" s="9"/>
+      <c r="E271" s="5">
+        <v>1</v>
+      </c>
+      <c r="F271" s="6">
+        <v>2</v>
+      </c>
+      <c r="G271" s="6">
+        <v>3</v>
+      </c>
+      <c r="H271" s="6">
+        <v>4</v>
+      </c>
+      <c r="I271" s="6">
+        <v>5</v>
+      </c>
+      <c r="J271" s="9"/>
+      <c r="K271" s="9"/>
+      <c r="L271" s="9"/>
+      <c r="M271" s="9"/>
+      <c r="N271" s="9"/>
+      <c r="O271" s="9"/>
+      <c r="P271" s="9"/>
+      <c r="Q271" s="9"/>
+      <c r="R271" s="9"/>
+      <c r="S271" s="9"/>
+      <c r="T271" s="9"/>
+      <c r="U271" s="9"/>
+    </row>
+    <row r="272" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A272" s="10">
+        <v>4</v>
+      </c>
+      <c r="B272" s="11"/>
+      <c r="C272" s="12"/>
+      <c r="D272" s="12"/>
+      <c r="E272" s="12"/>
+      <c r="F272" s="13">
+        <v>1</v>
+      </c>
+      <c r="G272" s="14">
+        <v>2</v>
+      </c>
+      <c r="H272" s="14">
+        <v>3</v>
+      </c>
+      <c r="I272" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J272" s="14">
+        <v>4</v>
+      </c>
+      <c r="K272" s="12">
+        <v>5</v>
+      </c>
+      <c r="L272" s="9"/>
+      <c r="M272" s="9"/>
+      <c r="N272" s="9"/>
+      <c r="O272" s="9"/>
+      <c r="P272" s="9"/>
+      <c r="Q272" s="9"/>
+      <c r="R272" s="9"/>
+      <c r="S272" s="9"/>
+      <c r="T272" s="9"/>
+      <c r="U272" s="9"/>
+    </row>
+    <row r="273" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A273" s="37">
+        <v>5</v>
+      </c>
+      <c r="B273" s="38"/>
+      <c r="C273" s="39"/>
+      <c r="D273" s="39"/>
+      <c r="E273" s="39"/>
+      <c r="F273" s="39"/>
+      <c r="G273" s="39">
+        <v>1</v>
+      </c>
+      <c r="H273" s="39">
+        <v>2</v>
+      </c>
+      <c r="I273" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J273" s="39">
+        <v>3</v>
+      </c>
+      <c r="K273" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="L273" s="39">
+        <v>4</v>
+      </c>
+      <c r="M273" s="39">
+        <v>5</v>
+      </c>
+      <c r="N273" s="9"/>
+      <c r="O273" s="9"/>
+      <c r="P273" s="9"/>
+      <c r="Q273" s="9"/>
+      <c r="R273" s="9"/>
+      <c r="S273" s="9"/>
+      <c r="T273" s="9"/>
+      <c r="U273" s="9"/>
+    </row>
+    <row r="274" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A274" s="7">
+        <v>6</v>
+      </c>
+      <c r="B274" s="8"/>
+      <c r="C274" s="9"/>
+      <c r="D274" s="9"/>
+      <c r="E274" s="9"/>
+      <c r="F274" s="9"/>
+      <c r="G274" s="9"/>
+      <c r="H274" s="9">
+        <v>1</v>
+      </c>
+      <c r="I274" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J274" s="9">
+        <v>2</v>
+      </c>
+      <c r="K274" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L274" s="9">
+        <v>3</v>
+      </c>
+      <c r="M274" s="9">
+        <v>4</v>
+      </c>
+      <c r="N274" s="9">
+        <v>5</v>
+      </c>
+      <c r="O274" s="9"/>
+      <c r="P274" s="9"/>
+      <c r="Q274" s="9"/>
+      <c r="R274" s="9"/>
+      <c r="S274" s="9"/>
+      <c r="T274" s="9"/>
+      <c r="U274" s="9"/>
+    </row>
+    <row r="275" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A275" s="7">
+        <v>7</v>
+      </c>
+      <c r="B275" s="8"/>
+      <c r="C275" s="9"/>
+      <c r="D275" s="9"/>
+      <c r="E275" s="9"/>
+      <c r="F275" s="9"/>
+      <c r="G275" s="9"/>
+      <c r="H275" s="9"/>
+      <c r="I275" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J275" s="9">
+        <v>1</v>
+      </c>
+      <c r="K275" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L275" s="9">
+        <v>2</v>
+      </c>
+      <c r="M275" s="9">
+        <v>3</v>
+      </c>
+      <c r="N275" s="9">
+        <v>4</v>
+      </c>
+      <c r="O275" s="9">
+        <v>5</v>
+      </c>
+      <c r="P275" s="9"/>
+      <c r="Q275" s="9"/>
+      <c r="R275" s="9"/>
+      <c r="S275" s="9"/>
+      <c r="T275" s="9"/>
+      <c r="U275" s="9"/>
+    </row>
+    <row r="278" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A278" s="30">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="279" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A279" s="1"/>
+      <c r="B279" s="2">
+        <v>1</v>
+      </c>
+      <c r="C279" s="3">
+        <v>2</v>
+      </c>
+      <c r="D279" s="3">
+        <v>3</v>
+      </c>
+      <c r="E279" s="3">
+        <v>4</v>
+      </c>
+      <c r="F279" s="3">
+        <v>5</v>
+      </c>
+      <c r="G279" s="3">
+        <v>6</v>
+      </c>
+      <c r="H279" s="3">
+        <v>7</v>
+      </c>
+      <c r="I279" s="3">
+        <v>8</v>
+      </c>
+      <c r="J279" s="3">
+        <v>9</v>
+      </c>
+      <c r="K279" s="3">
+        <v>10</v>
+      </c>
+      <c r="L279" s="3">
+        <v>11</v>
+      </c>
+      <c r="M279" s="3">
+        <v>12</v>
+      </c>
+      <c r="N279" s="3">
+        <v>13</v>
+      </c>
+      <c r="O279" s="3">
+        <v>14</v>
+      </c>
+      <c r="P279" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q279" s="3">
+        <v>16</v>
+      </c>
+      <c r="R279" s="3">
+        <v>17</v>
+      </c>
+      <c r="S279" s="3">
+        <v>18</v>
+      </c>
+      <c r="T279" s="3">
+        <v>19</v>
+      </c>
+      <c r="U279" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="280" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A280" s="4">
+        <v>0</v>
+      </c>
+      <c r="B280" s="5">
+        <v>1</v>
+      </c>
+      <c r="C280" s="6">
+        <v>2</v>
+      </c>
+      <c r="D280" s="6">
+        <v>3</v>
+      </c>
+      <c r="E280" s="6">
+        <v>4</v>
+      </c>
+      <c r="F280" s="6">
+        <v>5</v>
+      </c>
+      <c r="G280" s="6"/>
+      <c r="H280" s="6"/>
+      <c r="I280" s="6"/>
+      <c r="J280" s="6"/>
+      <c r="K280" s="6"/>
+      <c r="L280" s="6"/>
+      <c r="M280" s="6"/>
+      <c r="N280" s="6"/>
+      <c r="O280" s="6"/>
+      <c r="P280" s="6"/>
+      <c r="Q280" s="6"/>
+      <c r="R280" s="6"/>
+      <c r="S280" s="6"/>
+      <c r="T280" s="6"/>
+      <c r="U280" s="6"/>
+    </row>
+    <row r="281" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A281" s="7">
+        <v>1</v>
+      </c>
+      <c r="B281" s="8"/>
+      <c r="C281" s="5">
+        <v>1</v>
+      </c>
+      <c r="D281" s="6">
+        <v>2</v>
+      </c>
+      <c r="E281" s="6">
+        <v>3</v>
+      </c>
+      <c r="F281" s="6">
+        <v>4</v>
+      </c>
+      <c r="G281" s="6">
+        <v>5</v>
+      </c>
+      <c r="H281" s="9"/>
+      <c r="I281" s="9"/>
+      <c r="J281" s="9"/>
+      <c r="K281" s="9"/>
+      <c r="L281" s="9"/>
+      <c r="M281" s="9"/>
+      <c r="N281" s="9"/>
+      <c r="O281" s="9"/>
+      <c r="P281" s="9"/>
+      <c r="Q281" s="9"/>
+      <c r="R281" s="9"/>
+      <c r="S281" s="9"/>
+      <c r="T281" s="9"/>
+      <c r="U281" s="9"/>
+    </row>
+    <row r="282" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A282" s="7">
+        <v>2</v>
+      </c>
+      <c r="B282" s="8"/>
+      <c r="C282" s="9"/>
+      <c r="D282" s="5">
+        <v>1</v>
+      </c>
+      <c r="E282" s="6">
+        <v>2</v>
+      </c>
+      <c r="F282" s="6">
+        <v>3</v>
+      </c>
+      <c r="G282" s="6">
+        <v>4</v>
+      </c>
+      <c r="H282" s="6">
+        <v>5</v>
+      </c>
+      <c r="I282" s="9"/>
+      <c r="J282" s="9"/>
+      <c r="K282" s="9"/>
+      <c r="L282" s="9"/>
+      <c r="M282" s="9"/>
+      <c r="N282" s="9"/>
+      <c r="O282" s="9"/>
+      <c r="P282" s="9"/>
+      <c r="Q282" s="9"/>
+      <c r="R282" s="9"/>
+      <c r="S282" s="9"/>
+      <c r="T282" s="9"/>
+      <c r="U282" s="9"/>
+    </row>
+    <row r="283" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A283" s="7">
+        <v>3</v>
+      </c>
+      <c r="B283" s="8"/>
+      <c r="C283" s="9"/>
+      <c r="D283" s="9"/>
+      <c r="E283" s="5">
+        <v>1</v>
+      </c>
+      <c r="F283" s="6">
+        <v>2</v>
+      </c>
+      <c r="G283" s="6">
+        <v>3</v>
+      </c>
+      <c r="H283" s="6">
+        <v>4</v>
+      </c>
+      <c r="I283" s="6">
+        <v>5</v>
+      </c>
+      <c r="J283" s="9"/>
+      <c r="K283" s="9"/>
+      <c r="L283" s="9"/>
+      <c r="M283" s="9"/>
+      <c r="N283" s="9"/>
+      <c r="O283" s="9"/>
+      <c r="P283" s="9"/>
+      <c r="Q283" s="9"/>
+      <c r="R283" s="9"/>
+      <c r="S283" s="9"/>
+      <c r="T283" s="9"/>
+      <c r="U283" s="9"/>
+    </row>
+    <row r="284" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A284" s="10">
+        <v>4</v>
+      </c>
+      <c r="B284" s="11"/>
+      <c r="C284" s="12"/>
+      <c r="D284" s="12"/>
+      <c r="E284" s="12"/>
+      <c r="F284" s="13">
+        <v>1</v>
+      </c>
+      <c r="G284" s="14">
+        <v>2</v>
+      </c>
+      <c r="H284" s="14">
+        <v>3</v>
+      </c>
+      <c r="I284" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J284" s="14">
+        <v>4</v>
+      </c>
+      <c r="K284" s="12">
+        <v>5</v>
+      </c>
+      <c r="L284" s="9"/>
+      <c r="M284" s="9"/>
+      <c r="N284" s="9"/>
+      <c r="O284" s="9"/>
+      <c r="P284" s="9"/>
+      <c r="Q284" s="9"/>
+      <c r="R284" s="9"/>
+      <c r="S284" s="9"/>
+      <c r="T284" s="9"/>
+      <c r="U284" s="9"/>
+    </row>
+    <row r="285" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A285" s="20">
+        <v>5</v>
+      </c>
+      <c r="B285" s="21"/>
+      <c r="C285" s="22"/>
+      <c r="D285" s="22"/>
+      <c r="E285" s="22"/>
+      <c r="F285" s="22"/>
+      <c r="G285" s="22">
+        <v>1</v>
+      </c>
+      <c r="H285" s="22">
+        <v>2</v>
+      </c>
+      <c r="I285" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J285" s="22">
+        <v>3</v>
+      </c>
+      <c r="K285" s="22">
+        <v>4</v>
+      </c>
+      <c r="L285" s="22">
+        <v>5</v>
+      </c>
+      <c r="M285" s="9"/>
+      <c r="N285" s="9"/>
+      <c r="O285" s="9"/>
+      <c r="P285" s="9"/>
+      <c r="Q285" s="9"/>
+      <c r="R285" s="9"/>
+      <c r="S285" s="9"/>
+      <c r="T285" s="9"/>
+      <c r="U285" s="9"/>
+    </row>
+    <row r="286" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A286" s="37">
+        <v>6</v>
+      </c>
+      <c r="B286" s="38"/>
+      <c r="C286" s="39"/>
+      <c r="D286" s="39"/>
+      <c r="E286" s="39"/>
+      <c r="F286" s="39"/>
+      <c r="G286" s="39"/>
+      <c r="H286" s="39">
+        <v>1</v>
+      </c>
+      <c r="I286" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J286" s="39">
+        <v>2</v>
+      </c>
+      <c r="K286" s="39">
+        <v>3</v>
+      </c>
+      <c r="L286" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="M286" s="39">
+        <v>4</v>
+      </c>
+      <c r="N286" s="39">
+        <v>5</v>
+      </c>
+      <c r="O286" s="9"/>
+      <c r="P286" s="9"/>
+      <c r="Q286" s="9"/>
+      <c r="R286" s="9"/>
+      <c r="S286" s="9"/>
+      <c r="T286" s="9"/>
+      <c r="U286" s="9"/>
+    </row>
+    <row r="287" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A287" s="7">
+        <v>7</v>
+      </c>
+      <c r="B287" s="8"/>
+      <c r="C287" s="9"/>
+      <c r="D287" s="9"/>
+      <c r="E287" s="9"/>
+      <c r="F287" s="9"/>
+      <c r="G287" s="9"/>
+      <c r="H287" s="9"/>
+      <c r="I287" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J287" s="9">
+        <v>1</v>
+      </c>
+      <c r="K287" s="9">
+        <v>2</v>
+      </c>
+      <c r="L287" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M287" s="9">
+        <v>3</v>
+      </c>
+      <c r="N287" s="9">
+        <v>4</v>
+      </c>
+      <c r="O287" s="9">
+        <v>5</v>
+      </c>
+      <c r="P287" s="9"/>
+      <c r="Q287" s="9"/>
+      <c r="R287" s="9"/>
+      <c r="S287" s="9"/>
+      <c r="T287" s="9"/>
+      <c r="U287" s="9"/>
+    </row>
+    <row r="288" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A288" s="7">
+        <v>8</v>
+      </c>
+      <c r="B288" s="8"/>
+      <c r="C288" s="9"/>
+      <c r="D288" s="9"/>
+      <c r="E288" s="9"/>
+      <c r="F288" s="9"/>
+      <c r="G288" s="9"/>
+      <c r="H288" s="9"/>
+      <c r="I288" s="9"/>
+      <c r="J288" s="9"/>
+      <c r="K288" s="9">
+        <v>1</v>
+      </c>
+      <c r="L288" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="M288" s="9">
+        <v>2</v>
+      </c>
+      <c r="N288" s="9">
+        <v>3</v>
+      </c>
+      <c r="O288" s="9">
+        <v>4</v>
+      </c>
+      <c r="P288" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q288" s="9"/>
+      <c r="R288" s="9"/>
+      <c r="S288" s="9"/>
+      <c r="T288" s="9"/>
+      <c r="U288" s="9"/>
+    </row>
+    <row r="291" spans="1:21" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A291" s="30">
+        <v>2.15</v>
+      </c>
+    </row>
+    <row r="292" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A292" s="1"/>
+      <c r="B292" s="2">
+        <v>1</v>
+      </c>
+      <c r="C292" s="3">
+        <v>2</v>
+      </c>
+      <c r="D292" s="3">
+        <v>3</v>
+      </c>
+      <c r="E292" s="3">
+        <v>4</v>
+      </c>
+      <c r="F292" s="3">
+        <v>5</v>
+      </c>
+      <c r="G292" s="3">
+        <v>6</v>
+      </c>
+      <c r="H292" s="3">
+        <v>7</v>
+      </c>
+      <c r="I292" s="3">
+        <v>8</v>
+      </c>
+      <c r="J292" s="3">
+        <v>9</v>
+      </c>
+      <c r="K292" s="3">
+        <v>10</v>
+      </c>
+      <c r="L292" s="3">
+        <v>11</v>
+      </c>
+      <c r="M292" s="3">
+        <v>12</v>
+      </c>
+      <c r="N292" s="3">
+        <v>13</v>
+      </c>
+      <c r="O292" s="3">
+        <v>14</v>
+      </c>
+      <c r="P292" s="3">
+        <v>15</v>
+      </c>
+      <c r="Q292" s="3">
+        <v>16</v>
+      </c>
+      <c r="R292" s="3">
+        <v>17</v>
+      </c>
+      <c r="S292" s="3">
+        <v>18</v>
+      </c>
+      <c r="T292" s="3">
+        <v>19</v>
+      </c>
+      <c r="U292" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="293" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A293" s="4">
+        <v>0</v>
+      </c>
+      <c r="B293" s="5">
+        <v>1</v>
+      </c>
+      <c r="C293" s="6">
+        <v>2</v>
+      </c>
+      <c r="D293" s="6">
+        <v>3</v>
+      </c>
+      <c r="E293" s="6">
+        <v>4</v>
+      </c>
+      <c r="F293" s="6">
+        <v>5</v>
+      </c>
+      <c r="G293" s="6"/>
+      <c r="H293" s="6"/>
+      <c r="I293" s="6"/>
+      <c r="J293" s="6"/>
+      <c r="K293" s="6"/>
+      <c r="L293" s="6"/>
+      <c r="M293" s="6"/>
+      <c r="N293" s="6"/>
+      <c r="O293" s="6"/>
+      <c r="P293" s="6"/>
+      <c r="Q293" s="6"/>
+      <c r="R293" s="6"/>
+      <c r="S293" s="6"/>
+      <c r="T293" s="6"/>
+      <c r="U293" s="6"/>
+    </row>
+    <row r="294" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A294" s="7">
+        <v>1</v>
+      </c>
+      <c r="B294" s="8"/>
+      <c r="C294" s="5">
+        <v>1</v>
+      </c>
+      <c r="D294" s="6">
+        <v>2</v>
+      </c>
+      <c r="E294" s="6">
+        <v>3</v>
+      </c>
+      <c r="F294" s="6">
+        <v>4</v>
+      </c>
+      <c r="G294" s="6">
+        <v>5</v>
+      </c>
+      <c r="H294" s="9"/>
+      <c r="I294" s="9"/>
+      <c r="J294" s="9"/>
+      <c r="K294" s="9"/>
+      <c r="L294" s="9"/>
+      <c r="M294" s="9"/>
+      <c r="N294" s="9"/>
+      <c r="O294" s="9"/>
+      <c r="P294" s="9"/>
+      <c r="Q294" s="9"/>
+      <c r="R294" s="9"/>
+      <c r="S294" s="9"/>
+      <c r="T294" s="9"/>
+      <c r="U294" s="9"/>
+    </row>
+    <row r="295" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A295" s="7">
+        <v>2</v>
+      </c>
+      <c r="B295" s="8"/>
+      <c r="C295" s="9"/>
+      <c r="D295" s="5">
+        <v>1</v>
+      </c>
+      <c r="E295" s="6">
+        <v>2</v>
+      </c>
+      <c r="F295" s="6">
+        <v>3</v>
+      </c>
+      <c r="G295" s="6">
+        <v>4</v>
+      </c>
+      <c r="H295" s="6">
+        <v>5</v>
+      </c>
+      <c r="I295" s="9"/>
+      <c r="J295" s="9"/>
+      <c r="K295" s="9"/>
+      <c r="L295" s="9"/>
+      <c r="M295" s="9"/>
+      <c r="N295" s="9"/>
+      <c r="O295" s="9"/>
+      <c r="P295" s="9"/>
+      <c r="Q295" s="9"/>
+      <c r="R295" s="9"/>
+      <c r="S295" s="9"/>
+      <c r="T295" s="9"/>
+      <c r="U295" s="9"/>
+    </row>
+    <row r="296" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A296" s="7">
+        <v>3</v>
+      </c>
+      <c r="B296" s="8"/>
+      <c r="C296" s="9"/>
+      <c r="D296" s="9"/>
+      <c r="E296" s="5">
+        <v>1</v>
+      </c>
+      <c r="F296" s="6">
+        <v>2</v>
+      </c>
+      <c r="G296" s="6">
+        <v>3</v>
+      </c>
+      <c r="H296" s="6">
+        <v>4</v>
+      </c>
+      <c r="I296" s="6">
+        <v>5</v>
+      </c>
+      <c r="J296" s="9"/>
+      <c r="K296" s="9"/>
+      <c r="L296" s="9"/>
+      <c r="M296" s="9"/>
+      <c r="N296" s="9"/>
+      <c r="O296" s="9"/>
+      <c r="P296" s="9"/>
+      <c r="Q296" s="9"/>
+      <c r="R296" s="9"/>
+      <c r="S296" s="9"/>
+      <c r="T296" s="9"/>
+      <c r="U296" s="9"/>
+    </row>
+    <row r="297" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A297" s="10">
+        <v>4</v>
+      </c>
+      <c r="B297" s="11"/>
+      <c r="C297" s="12"/>
+      <c r="D297" s="12"/>
+      <c r="E297" s="12"/>
+      <c r="F297" s="13">
+        <v>1</v>
+      </c>
+      <c r="G297" s="14">
+        <v>2</v>
+      </c>
+      <c r="H297" s="14">
+        <v>3</v>
+      </c>
+      <c r="I297" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J297" s="14">
+        <v>4</v>
+      </c>
+      <c r="K297" s="12">
+        <v>5</v>
+      </c>
+      <c r="L297" s="9"/>
+      <c r="M297" s="9"/>
+      <c r="N297" s="9"/>
+      <c r="O297" s="9"/>
+      <c r="P297" s="9"/>
+      <c r="Q297" s="9"/>
+      <c r="R297" s="9"/>
+      <c r="S297" s="9"/>
+      <c r="T297" s="9"/>
+      <c r="U297" s="9"/>
+    </row>
+    <row r="298" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A298" s="20">
+        <v>5</v>
+      </c>
+      <c r="B298" s="21"/>
+      <c r="C298" s="22"/>
+      <c r="D298" s="22"/>
+      <c r="E298" s="22"/>
+      <c r="F298" s="22"/>
+      <c r="G298" s="22">
+        <v>1</v>
+      </c>
+      <c r="H298" s="22">
+        <v>2</v>
+      </c>
+      <c r="I298" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J298" s="22">
+        <v>3</v>
+      </c>
+      <c r="K298" s="22">
+        <v>4</v>
+      </c>
+      <c r="L298" s="22">
+        <v>5</v>
+      </c>
+      <c r="M298" s="9"/>
+      <c r="N298" s="9"/>
+      <c r="O298" s="9"/>
+      <c r="P298" s="9"/>
+      <c r="Q298" s="9"/>
+      <c r="R298" s="9"/>
+      <c r="S298" s="9"/>
+      <c r="T298" s="9"/>
+      <c r="U298" s="9"/>
+    </row>
+    <row r="299" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A299" s="7">
+        <v>6</v>
+      </c>
+      <c r="B299" s="8"/>
+      <c r="C299" s="9"/>
+      <c r="D299" s="9"/>
+      <c r="E299" s="9"/>
+      <c r="F299" s="9"/>
+      <c r="G299" s="9"/>
+      <c r="H299" s="9">
+        <v>1</v>
+      </c>
+      <c r="I299" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="J299" s="9">
+        <v>2</v>
+      </c>
+      <c r="K299" s="9">
+        <v>3</v>
+      </c>
+      <c r="L299" s="9">
+        <v>4</v>
+      </c>
+      <c r="M299" s="9">
+        <v>5</v>
+      </c>
+      <c r="N299" s="9"/>
+      <c r="O299" s="9"/>
+      <c r="Q299" s="9"/>
+      <c r="R299" s="9"/>
+      <c r="S299" s="9"/>
+      <c r="T299" s="9"/>
+      <c r="U299" s="9"/>
+    </row>
+    <row r="300" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A300" s="37">
+        <v>7</v>
+      </c>
+      <c r="B300" s="38"/>
+      <c r="C300" s="39"/>
+      <c r="D300" s="39"/>
+      <c r="E300" s="39"/>
+      <c r="F300" s="39"/>
+      <c r="G300" s="39"/>
+      <c r="H300" s="39"/>
+      <c r="I300" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="J300" s="39">
+        <v>1</v>
+      </c>
+      <c r="K300" s="39">
+        <v>2</v>
+      </c>
+      <c r="L300" s="39">
+        <v>3</v>
+      </c>
+      <c r="M300" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="N300" s="39">
+        <v>4</v>
+      </c>
+      <c r="O300" s="39">
+        <v>5</v>
+      </c>
+      <c r="P300" s="9"/>
+      <c r="Q300" s="9"/>
+      <c r="R300" s="9"/>
+      <c r="S300" s="9"/>
+      <c r="T300" s="9"/>
+      <c r="U300" s="9"/>
+    </row>
+    <row r="301" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A301" s="7">
+        <v>8</v>
+      </c>
+      <c r="B301" s="8"/>
+      <c r="C301" s="9"/>
+      <c r="D301" s="9"/>
+      <c r="E301" s="9"/>
+      <c r="F301" s="9"/>
+      <c r="G301" s="9"/>
+      <c r="H301" s="9"/>
+      <c r="I301" s="9"/>
+      <c r="J301" s="9"/>
+      <c r="K301" s="9">
+        <v>1</v>
+      </c>
+      <c r="L301" s="9">
+        <v>2</v>
+      </c>
+      <c r="M301" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N301" s="9">
+        <v>3</v>
+      </c>
+      <c r="O301" s="9">
+        <v>4</v>
+      </c>
+      <c r="P301" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q301" s="9"/>
+      <c r="R301" s="9"/>
+      <c r="S301" s="9"/>
+      <c r="T301" s="9"/>
+      <c r="U301" s="9"/>
+    </row>
+    <row r="302" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A302" s="7">
+        <v>9</v>
+      </c>
+      <c r="B302" s="8"/>
+      <c r="C302" s="9"/>
+      <c r="D302" s="9"/>
+      <c r="E302" s="9"/>
+      <c r="F302" s="9"/>
+      <c r="G302" s="9"/>
+      <c r="H302" s="9"/>
+      <c r="I302" s="9"/>
+      <c r="J302" s="9"/>
+      <c r="K302" s="9"/>
+      <c r="L302" s="9">
+        <v>1</v>
+      </c>
+      <c r="M302" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N302" s="9">
+        <v>2</v>
+      </c>
+      <c r="O302" s="9">
+        <v>3</v>
+      </c>
+      <c r="P302" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q302" s="9">
+        <v>5</v>
+      </c>
+      <c r="R302" s="9"/>
+      <c r="S302" s="9"/>
+      <c r="T302" s="9"/>
+      <c r="U302" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAAB599-C37A-4392-8901-12901559E5CE}">
+  <dimension ref="B3:AO25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="2:41" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="4" spans="2:41" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7</v>
+      </c>
+      <c r="J4" s="3">
+        <v>8</v>
+      </c>
+      <c r="K4" s="3">
+        <v>9</v>
+      </c>
+      <c r="L4" s="3">
+        <v>10</v>
+      </c>
+      <c r="M4" s="3">
+        <v>11</v>
+      </c>
+      <c r="N4" s="3">
+        <v>12</v>
+      </c>
+      <c r="O4" s="3">
+        <v>13</v>
+      </c>
+      <c r="P4" s="3">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>15</v>
+      </c>
+      <c r="R4" s="3">
+        <v>16</v>
+      </c>
+      <c r="S4" s="3">
+        <v>17</v>
+      </c>
+      <c r="T4" s="3">
+        <v>18</v>
+      </c>
+      <c r="U4" s="3">
+        <v>19</v>
+      </c>
+      <c r="V4" s="3">
+        <v>20</v>
+      </c>
+      <c r="W4" s="3">
+        <v>21</v>
+      </c>
+      <c r="X4" s="3">
+        <v>22</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>23</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>24</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>25</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>26</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>27</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>29</v>
+      </c>
+      <c r="AF4" s="3">
+        <v>30</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>31</v>
+      </c>
+      <c r="AH4" s="3">
+        <v>32</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>33</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>34</v>
+      </c>
+      <c r="AK4" s="3">
+        <v>35</v>
+      </c>
+      <c r="AL4" s="3">
+        <v>36</v>
+      </c>
+      <c r="AM4" s="3">
+        <v>37</v>
+      </c>
+      <c r="AN4" s="3">
+        <v>38</v>
+      </c>
+      <c r="AO4" s="3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="4">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+      <c r="F5" s="6">
+        <v>4</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="9"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="9"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="9"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9"/>
+      <c r="AI5" s="9"/>
+      <c r="AJ5" s="9"/>
+      <c r="AK5" s="9"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="9"/>
+      <c r="AN5" s="9"/>
+      <c r="AO5" s="9"/>
+    </row>
+    <row r="6" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>3</v>
+      </c>
+      <c r="G6" s="6">
+        <v>4</v>
+      </c>
+      <c r="H6" s="6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="9"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="9"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
+      <c r="AK6" s="9"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="9"/>
+      <c r="AN6" s="9"/>
+      <c r="AO6" s="9"/>
+    </row>
+    <row r="7" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>3</v>
+      </c>
+      <c r="H7" s="6">
+        <v>4</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
+      <c r="U7" s="9"/>
+      <c r="V7" s="9"/>
+      <c r="W7" s="9"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="9"/>
+      <c r="Z7" s="9"/>
+      <c r="AA7" s="9"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="9"/>
+      <c r="AF7" s="9"/>
+      <c r="AG7" s="9"/>
+      <c r="AH7" s="9"/>
+      <c r="AI7" s="9"/>
+      <c r="AJ7" s="9"/>
+      <c r="AK7" s="9"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="9"/>
+      <c r="AN7" s="9"/>
+      <c r="AO7" s="9"/>
+    </row>
+    <row r="8" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="7">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6">
+        <v>3</v>
+      </c>
+      <c r="J8" s="6">
+        <v>4</v>
+      </c>
+      <c r="K8" s="6">
+        <v>5</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="9"/>
+      <c r="Y8" s="9"/>
+      <c r="Z8" s="9"/>
+      <c r="AA8" s="9"/>
+      <c r="AB8" s="9"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="9"/>
+      <c r="AF8" s="9"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="9"/>
+      <c r="AI8" s="9"/>
+      <c r="AJ8" s="9"/>
+      <c r="AK8" s="9"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="9"/>
+      <c r="AN8" s="9"/>
+      <c r="AO8" s="9"/>
+    </row>
+    <row r="9" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="20">
+        <v>4</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="9"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
+      <c r="AB9" s="9"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="9"/>
+      <c r="AF9" s="9"/>
+      <c r="AG9" s="9"/>
+      <c r="AH9" s="9"/>
+      <c r="AI9" s="9"/>
+      <c r="AJ9" s="9"/>
+      <c r="AK9" s="9"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="9"/>
+      <c r="AN9" s="9"/>
+      <c r="AO9" s="9"/>
+    </row>
+    <row r="10" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="20">
+        <v>5</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="9"/>
+      <c r="V10" s="9"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="9"/>
+      <c r="Y10" s="9"/>
+      <c r="Z10" s="9"/>
+      <c r="AA10" s="9"/>
+      <c r="AB10" s="9"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="9"/>
+      <c r="AF10" s="9"/>
+      <c r="AG10" s="9"/>
+      <c r="AH10" s="9"/>
+      <c r="AI10" s="9"/>
+      <c r="AJ10" s="9"/>
+      <c r="AK10" s="9"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="9"/>
+      <c r="AN10" s="9"/>
+      <c r="AO10" s="9"/>
+    </row>
+    <row r="11" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="9"/>
+      <c r="AA11" s="9"/>
+      <c r="AB11" s="9"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="9"/>
+      <c r="AF11" s="9"/>
+      <c r="AG11" s="9"/>
+      <c r="AH11" s="9"/>
+      <c r="AI11" s="9"/>
+      <c r="AJ11" s="9"/>
+      <c r="AK11" s="9"/>
+      <c r="AL11" s="9"/>
+      <c r="AM11" s="9"/>
+      <c r="AN11" s="9"/>
+      <c r="AO11" s="9"/>
+    </row>
+    <row r="12" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="20">
+        <v>7</v>
+      </c>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
+      <c r="AG12" s="9"/>
+      <c r="AH12" s="9"/>
+      <c r="AI12" s="9"/>
+      <c r="AJ12" s="9"/>
+      <c r="AK12" s="9"/>
+      <c r="AL12" s="9"/>
+      <c r="AM12" s="9"/>
+      <c r="AN12" s="9"/>
+      <c r="AO12" s="9"/>
+    </row>
+    <row r="13" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="7">
+        <v>8</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="9"/>
+      <c r="V13" s="9"/>
+      <c r="W13" s="9"/>
+      <c r="X13" s="9"/>
+      <c r="Y13" s="9"/>
+      <c r="Z13" s="9"/>
+      <c r="AA13" s="9"/>
+      <c r="AB13" s="9"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="9"/>
+      <c r="AF13" s="9"/>
+      <c r="AG13" s="9"/>
+      <c r="AH13" s="9"/>
+      <c r="AI13" s="9"/>
+      <c r="AJ13" s="9"/>
+      <c r="AK13" s="9"/>
+      <c r="AL13" s="9"/>
+      <c r="AM13" s="9"/>
+      <c r="AN13" s="9"/>
+      <c r="AO13" s="9"/>
+    </row>
+    <row r="14" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="7">
+        <v>9</v>
+      </c>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+      <c r="AG14" s="9"/>
+      <c r="AH14" s="9"/>
+      <c r="AI14" s="9"/>
+      <c r="AJ14" s="9"/>
+      <c r="AK14" s="9"/>
+      <c r="AL14" s="9"/>
+      <c r="AM14" s="9"/>
+      <c r="AN14" s="9"/>
+      <c r="AO14" s="9"/>
+    </row>
+    <row r="15" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="7">
+        <v>10</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="9"/>
+      <c r="AI15" s="9"/>
+      <c r="AJ15" s="9"/>
+      <c r="AK15" s="9"/>
+      <c r="AL15" s="9"/>
+      <c r="AM15" s="9"/>
+      <c r="AN15" s="9"/>
+      <c r="AO15" s="9"/>
+    </row>
+    <row r="16" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B16" s="7">
+        <v>11</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
+      <c r="Y16" s="9"/>
+      <c r="Z16" s="9"/>
+      <c r="AA16" s="9"/>
+      <c r="AB16" s="9"/>
+      <c r="AC16" s="9"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="9"/>
+      <c r="AF16" s="9"/>
+      <c r="AG16" s="9"/>
+      <c r="AH16" s="9"/>
+      <c r="AI16" s="9"/>
+      <c r="AJ16" s="9"/>
+      <c r="AK16" s="9"/>
+      <c r="AL16" s="9"/>
+      <c r="AM16" s="9"/>
+      <c r="AN16" s="9"/>
+      <c r="AO16" s="9"/>
+    </row>
+    <row r="17" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B17" s="7">
+        <v>12</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
+      <c r="Z17" s="9"/>
+      <c r="AA17" s="9"/>
+      <c r="AB17" s="9"/>
+      <c r="AC17" s="9"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="9"/>
+      <c r="AF17" s="9"/>
+      <c r="AG17" s="9"/>
+      <c r="AH17" s="9"/>
+      <c r="AI17" s="9"/>
+      <c r="AJ17" s="9"/>
+      <c r="AK17" s="9"/>
+      <c r="AL17" s="9"/>
+      <c r="AM17" s="9"/>
+      <c r="AN17" s="9"/>
+      <c r="AO17" s="9"/>
+    </row>
+    <row r="18" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B18" s="7">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+      <c r="AG18" s="9"/>
+      <c r="AH18" s="9"/>
+      <c r="AI18" s="9"/>
+      <c r="AJ18" s="9"/>
+      <c r="AK18" s="9"/>
+      <c r="AL18" s="9"/>
+      <c r="AM18" s="9"/>
+      <c r="AN18" s="9"/>
+      <c r="AO18" s="9"/>
+    </row>
+    <row r="19" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B19" s="7">
+        <v>14</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
+      <c r="AG19" s="9"/>
+      <c r="AH19" s="9"/>
+      <c r="AI19" s="9"/>
+      <c r="AJ19" s="9"/>
+      <c r="AK19" s="9"/>
+      <c r="AL19" s="9"/>
+      <c r="AM19" s="9"/>
+      <c r="AN19" s="9"/>
+      <c r="AO19" s="9"/>
+    </row>
+    <row r="20" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B20" s="7">
+        <v>15</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+      <c r="Z20" s="9"/>
+      <c r="AA20" s="9"/>
+      <c r="AB20" s="9"/>
+      <c r="AC20" s="9"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="9"/>
+      <c r="AF20" s="9"/>
+      <c r="AG20" s="9"/>
+      <c r="AH20" s="9"/>
+      <c r="AI20" s="9"/>
+      <c r="AJ20" s="9"/>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
+      <c r="AM20" s="9"/>
+      <c r="AN20" s="9"/>
+      <c r="AO20" s="9"/>
+    </row>
+    <row r="21" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B21" s="7">
+        <v>16</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+      <c r="AG21" s="9"/>
+      <c r="AH21" s="9"/>
+      <c r="AI21" s="9"/>
+      <c r="AJ21" s="9"/>
+      <c r="AK21" s="9"/>
+      <c r="AL21" s="9"/>
+      <c r="AM21" s="9"/>
+      <c r="AN21" s="9"/>
+      <c r="AO21" s="9"/>
+    </row>
+    <row r="22" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="7">
+        <v>17</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
+      <c r="AG22" s="9"/>
+      <c r="AH22" s="9"/>
+      <c r="AI22" s="9"/>
+      <c r="AJ22" s="9"/>
+      <c r="AK22" s="9"/>
+      <c r="AL22" s="9"/>
+      <c r="AM22" s="9"/>
+      <c r="AN22" s="9"/>
+      <c r="AO22" s="9"/>
+    </row>
+    <row r="23" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B23" s="7">
+        <v>18</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="9"/>
+      <c r="Z23" s="9"/>
+      <c r="AA23" s="9"/>
+      <c r="AB23" s="9"/>
+      <c r="AC23" s="9"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="9"/>
+      <c r="AF23" s="9"/>
+      <c r="AG23" s="9"/>
+      <c r="AH23" s="9"/>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
+      <c r="AL23" s="9"/>
+      <c r="AM23" s="9"/>
+      <c r="AN23" s="9"/>
+      <c r="AO23" s="9"/>
+    </row>
+    <row r="24" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="7">
+        <v>19</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+      <c r="AG24" s="9"/>
+      <c r="AH24" s="9"/>
+      <c r="AI24" s="9"/>
+      <c r="AJ24" s="9"/>
+      <c r="AK24" s="9"/>
+      <c r="AL24" s="9"/>
+      <c r="AM24" s="9"/>
+      <c r="AN24" s="9"/>
+      <c r="AO24" s="9"/>
+    </row>
+    <row r="25" spans="2:41" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B25" s="7">
+        <v>20</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
+      <c r="AG25" s="9"/>
+      <c r="AH25" s="9"/>
+      <c r="AI25" s="9"/>
+      <c r="AJ25" s="9"/>
+      <c r="AK25" s="9"/>
+      <c r="AL25" s="9"/>
+      <c r="AM25" s="9"/>
+      <c r="AN25" s="9"/>
+      <c r="AO25" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>